<commit_message>
modyfikacja wartości współczynników po zmianie rezystorów w płycie głównej
</commit_message>
<xml_diff>
--- a/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
+++ b/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Glowna AC" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
   <si>
     <t>in</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Zakres</t>
+  </si>
+  <si>
+    <t>analog In karty</t>
   </si>
 </sst>
 </file>
@@ -169,11 +172,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90622592"/>
-        <c:axId val="91513216"/>
+        <c:axId val="80726656"/>
+        <c:axId val="81092992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90622592"/>
+        <c:axId val="80726656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -183,12 +186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91513216"/>
+        <c:crossAx val="81092992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91513216"/>
+        <c:axId val="81092992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -199,14 +202,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90622592"/>
+        <c:crossAx val="80726656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -295,11 +297,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92750208"/>
-        <c:axId val="92751744"/>
+        <c:axId val="87152896"/>
+        <c:axId val="87158784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92750208"/>
+        <c:axId val="87152896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -309,12 +311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92751744"/>
+        <c:crossAx val="87158784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92751744"/>
+        <c:axId val="87158784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -325,14 +327,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92750208"/>
+        <c:crossAx val="87152896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -421,11 +422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91926912"/>
-        <c:axId val="91928448"/>
+        <c:axId val="87203840"/>
+        <c:axId val="87205376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91926912"/>
+        <c:axId val="87203840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,12 +436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91928448"/>
+        <c:crossAx val="87205376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91928448"/>
+        <c:axId val="87205376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,7 +452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91926912"/>
+        <c:crossAx val="87203840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -547,11 +548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91940352"/>
-        <c:axId val="91941888"/>
+        <c:axId val="87225472"/>
+        <c:axId val="87227008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91940352"/>
+        <c:axId val="87225472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,12 +562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91941888"/>
+        <c:crossAx val="87227008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91941888"/>
+        <c:axId val="87227008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91940352"/>
+        <c:crossAx val="87225472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -673,11 +674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92506752"/>
-        <c:axId val="92508544"/>
+        <c:axId val="86792448"/>
+        <c:axId val="86806528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92506752"/>
+        <c:axId val="86792448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,12 +688,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92508544"/>
+        <c:crossAx val="86806528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92508544"/>
+        <c:axId val="86806528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,7 +704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92506752"/>
+        <c:crossAx val="86792448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -799,11 +800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92835840"/>
-        <c:axId val="92837376"/>
+        <c:axId val="85176704"/>
+        <c:axId val="85178240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92835840"/>
+        <c:axId val="85176704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,12 +814,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92837376"/>
+        <c:crossAx val="85178240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92837376"/>
+        <c:axId val="85178240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,14 +830,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92835840"/>
+        <c:crossAx val="85176704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -925,11 +925,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92857472"/>
-        <c:axId val="92859008"/>
+        <c:axId val="85190144"/>
+        <c:axId val="85191680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92857472"/>
+        <c:axId val="85190144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,12 +939,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92859008"/>
+        <c:crossAx val="85191680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92859008"/>
+        <c:axId val="85191680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,14 +955,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92857472"/>
+        <c:crossAx val="85190144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1051,11 +1050,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92293376"/>
-        <c:axId val="92311552"/>
+        <c:axId val="85232256"/>
+        <c:axId val="85234048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92293376"/>
+        <c:axId val="85232256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,12 +1064,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92311552"/>
+        <c:crossAx val="85234048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92311552"/>
+        <c:axId val="85234048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,14 +1080,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92293376"/>
+        <c:crossAx val="85232256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1177,11 +1175,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92669824"/>
-        <c:axId val="92671360"/>
+        <c:axId val="85275008"/>
+        <c:axId val="85276544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92669824"/>
+        <c:axId val="85275008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,12 +1189,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92671360"/>
+        <c:crossAx val="85276544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92671360"/>
+        <c:axId val="85276544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1207,14 +1205,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92669824"/>
+        <c:crossAx val="85275008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1303,11 +1300,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92629248"/>
-        <c:axId val="92691072"/>
+        <c:axId val="85300736"/>
+        <c:axId val="85302272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92629248"/>
+        <c:axId val="85300736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,12 +1314,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92691072"/>
+        <c:crossAx val="85302272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92691072"/>
+        <c:axId val="85302272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,14 +1330,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92629248"/>
+        <c:crossAx val="85300736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1429,11 +1425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92788992"/>
-        <c:axId val="92790784"/>
+        <c:axId val="87046400"/>
+        <c:axId val="87048192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92788992"/>
+        <c:axId val="87046400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,12 +1439,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92790784"/>
+        <c:crossAx val="87048192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92790784"/>
+        <c:axId val="87048192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,14 +1455,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92788992"/>
+        <c:crossAx val="87046400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1555,11 +1550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92619136"/>
-        <c:axId val="92620672"/>
+        <c:axId val="87105536"/>
+        <c:axId val="87107072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92619136"/>
+        <c:axId val="87105536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,12 +1564,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92620672"/>
+        <c:crossAx val="87107072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92620672"/>
+        <c:axId val="87107072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,14 +1580,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92619136"/>
+        <c:crossAx val="87105536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1681,11 +1675,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92638592"/>
-        <c:axId val="92644480"/>
+        <c:axId val="87135360"/>
+        <c:axId val="87136896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92638592"/>
+        <c:axId val="87135360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,12 +1689,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92644480"/>
+        <c:crossAx val="87136896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92644480"/>
+        <c:axId val="87136896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,14 +1705,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92638592"/>
+        <c:crossAx val="87135360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2435,34 +2428,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:M18"/>
+  <dimension ref="A5:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2470,360 +2469,372 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3.5219999999999998</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.72640000000000005</v>
+        <v>4.367</v>
       </c>
       <c r="E7">
-        <f>D7/C7</f>
-        <v>0.20624645088018173</v>
+        <v>0.4304</v>
       </c>
       <c r="F7">
-        <f>C7/D7</f>
-        <v>4.8485682819383253</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" ref="G7:H7" si="0">AVERAGE(D7:D9)</f>
-        <v>0.43593333333333334</v>
+        <f>E7/D7</f>
+        <v>9.8557362033432558E-2</v>
+      </c>
+      <c r="G7">
+        <f>D7/E7</f>
+        <v>10.146375464684015</v>
       </c>
       <c r="H7" s="1">
+        <f t="shared" ref="H7:I7" si="0">AVERAGE(E7:E9)</f>
+        <v>0.22216666666666665</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0.20618961105914027</v>
-      </c>
-      <c r="I7">
-        <f t="array" ref="I7:J8">LINEST(C7:C9,D7:D9,TRUE,TRUE)</f>
-        <v>4.8478750540407471</v>
+        <v>9.8706932256084456E-2</v>
       </c>
       <c r="J7">
-        <v>6.1633477517020197E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8">
+        <f t="array" ref="J7:K8">LINEST(D7:D9,E7:E9,TRUE,TRUE)</f>
+        <v>10.151521388499894</v>
+      </c>
+      <c r="K7">
+        <v>-1.9963351450598132E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>2.1150000000000002</v>
-      </c>
       <c r="D8">
-        <v>0.43609999999999999</v>
+        <v>1.901</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E9" si="1">D8/C8</f>
-        <v>0.20619385342789595</v>
+        <v>0.18740000000000001</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F9" si="2">C8/D8</f>
-        <v>4.8498050905755568</v>
-      </c>
-      <c r="G8" s="1"/>
+        <f t="shared" ref="F8:F9" si="1">E8/D8</f>
+        <v>9.857969489742241E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G9" si="2">D8/E8</f>
+        <v>10.144076840981857</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8">
-        <v>6.7169996689801575E-4</v>
-      </c>
+      <c r="I8" s="1"/>
       <c r="J8">
-        <v>3.3336721768128922E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9">
+        <v>2.728204368011885E-3</v>
+      </c>
+      <c r="K8">
+        <v>7.433787211909268E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>0.70489999999999997</v>
-      </c>
       <c r="D9">
-        <v>0.14530000000000001</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
-        <v>0.20612852886934319</v>
+        <v>4.87E-2</v>
       </c>
       <c r="F9">
+        <f t="shared" si="1"/>
+        <v>9.8983739837398374E-2</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="2"/>
-        <v>4.8513420509291114</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>10.102669404517453</v>
+      </c>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>3.5219999999999998</v>
-      </c>
       <c r="D10">
-        <v>0.72409999999999997</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:E18" si="3">D10/C10</f>
-        <v>0.20559341283361726</v>
+        <v>0.4289</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F18" si="4">C10/D10</f>
-        <v>4.8639690650462644</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" ref="G10:H10" si="5">AVERAGE(D10:D12)</f>
-        <v>0.43443333333333339</v>
+        <f t="shared" ref="F10:F18" si="3">E10/D10</f>
+        <v>9.8236371965185532E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G18" si="4">D10/E10</f>
+        <v>10.179529027745394</v>
       </c>
       <c r="H10" s="1">
+        <f t="shared" ref="H10:I10" si="5">AVERAGE(E10:E12)</f>
+        <v>0.22123333333333337</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" si="5"/>
-        <v>0.20513964385143432</v>
-      </c>
-      <c r="I10">
-        <f t="array" ref="I10:J11">LINEST(C10:C12,D10:D12,TRUE,TRUE)</f>
-        <v>4.8558609895921343</v>
+        <v>9.8027552094332893E-2</v>
       </c>
       <c r="J10">
-        <v>5.0854574215235537E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11">
+        <f t="array" ref="J10:K11">LINEST(D10:D12,E10:E12,TRUE,TRUE)</f>
+        <v>10.172303196741696</v>
+      </c>
+      <c r="K10">
+        <v>2.8141227741786956E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="C11">
-        <v>2.1128999999999998</v>
-      </c>
       <c r="D11">
-        <v>0.43440000000000001</v>
+        <v>1.9012</v>
       </c>
       <c r="E11">
+        <v>0.1867</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="3"/>
-        <v>0.20559420701405653</v>
-      </c>
-      <c r="F11">
+        <v>9.8201136124552918E-2</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="4"/>
-        <v>4.8639502762430933</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>10.1831815747188</v>
+      </c>
       <c r="H11" s="1"/>
-      <c r="I11">
-        <v>4.6985467544241209E-3</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="J11">
-        <v>2.3240654527453418E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12">
+        <v>3.5620280101080503E-3</v>
+      </c>
+      <c r="K11">
+        <v>9.6706646399537612E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="C12">
-        <v>0.70899999999999996</v>
-      </c>
       <c r="D12">
-        <v>0.14480000000000001</v>
+        <v>0.49259999999999998</v>
       </c>
       <c r="E12">
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="3"/>
-        <v>0.20423131170662909</v>
-      </c>
-      <c r="F12">
+        <v>9.7645148193260242E-2</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="4"/>
-        <v>4.8964088397790047</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>10.241164241164242</v>
+      </c>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>3.5219999999999998</v>
-      </c>
       <c r="D13">
-        <v>0.72250000000000003</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="E13">
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="3"/>
-        <v>0.2051391254968768</v>
-      </c>
-      <c r="F13">
+        <v>9.8053137883646363E-2</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="4"/>
-        <v>4.8747404844290649</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" ref="G13:H13" si="6">AVERAGE(D13:D15)</f>
-        <v>0.43356666666666671</v>
+        <v>10.198551740247606</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" ref="H13:I13" si="6">AVERAGE(E13:E15)</f>
+        <v>0.30336666666666662</v>
+      </c>
+      <c r="I13" s="1">
         <f t="shared" si="6"/>
-        <v>0.20506394775582806</v>
-      </c>
-      <c r="I13">
-        <f t="array" ref="I13:J14">LINEST(C13:C15,D13:D15,TRUE,TRUE)</f>
-        <v>4.8738758916718119</v>
+        <v>0.14142242882053521</v>
       </c>
       <c r="J13">
-        <v>8.1654256749130738E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14">
+        <f t="array" ref="J13:K14">LINEST(D13:D15,E13:E15,TRUE,TRUE)</f>
+        <v>6.8309474156436458</v>
+      </c>
+      <c r="K13">
+        <v>0.18088491900757298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14">
         <v>2</v>
       </c>
-      <c r="C14">
-        <v>2.1150000000000002</v>
-      </c>
       <c r="D14">
+        <v>1.901</v>
+      </c>
+      <c r="E14">
         <v>0.43369999999999997</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="3"/>
-        <v>0.20505910165484631</v>
-      </c>
-      <c r="F14">
+        <v>0.2281430825881115</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="4"/>
-        <v>4.8766428406732771</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>4.383214203366383</v>
+      </c>
       <c r="H14" s="1"/>
-      <c r="I14">
-        <v>1.1491564208776337E-3</v>
-      </c>
+      <c r="I14" s="1"/>
       <c r="J14">
-        <v>5.6724662227225172E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15">
+        <v>5.6661812720707632</v>
+      </c>
+      <c r="K14">
+        <v>1.9998173602908687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="C15">
-        <v>0.70489999999999997</v>
-      </c>
       <c r="D15">
-        <v>0.14449999999999999</v>
+        <v>0.49249999999999999</v>
       </c>
       <c r="E15">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="3"/>
-        <v>0.20499361611576108</v>
-      </c>
-      <c r="F15">
+        <v>9.8071065989847717E-2</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="4"/>
-        <v>4.8782006920415224</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>10.196687370600413</v>
+      </c>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="C16">
-        <v>3.5230000000000001</v>
-      </c>
       <c r="D16">
-        <v>0.72399999999999998</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="E16">
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="3"/>
-        <v>0.20550667045131987</v>
-      </c>
-      <c r="F16">
+        <v>9.8327989005955116E-2</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="4"/>
-        <v>4.8660220994475143</v>
-      </c>
-      <c r="G16" s="1">
-        <f>AVERAGE(D16:D18)</f>
-        <v>0.43443333333333328</v>
+        <v>10.170044258094572</v>
       </c>
       <c r="H16" s="1">
         <f>AVERAGE(E16:E18)</f>
-        <v>0.20554749698147998</v>
-      </c>
-      <c r="I16">
-        <f t="array" ref="I16:J17">LINEST(C16:C18,D16:D18,TRUE,TRUE)</f>
-        <v>4.8663444480090279</v>
+        <v>0.42157</v>
+      </c>
+      <c r="I16" s="1">
+        <f>AVERAGE(F16:F18)</f>
+        <v>0.20354785230334607</v>
       </c>
       <c r="J16">
-        <v>-4.3557303005492543E-4</v>
-      </c>
-      <c r="L16">
+        <f t="array" ref="J16:K17">LINEST(D16:D18,E16:E18,TRUE,TRUE)</f>
+        <v>1.9958488766515854</v>
+      </c>
+      <c r="K16">
+        <v>1.4117099890699909</v>
+      </c>
+      <c r="M16">
         <v>4.8571215441004565</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>-1.55928106662655E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="C17">
-        <v>2.1131000000000002</v>
-      </c>
       <c r="D17">
-        <v>0.43440000000000001</v>
+        <v>1.9008</v>
       </c>
       <c r="E17">
+        <v>0.78700999999999999</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="3"/>
-        <v>0.20557474800056788</v>
-      </c>
-      <c r="F17">
+        <v>0.41404145622895622</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="4"/>
-        <v>4.8644106813996322</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>2.4152170874575929</v>
+      </c>
       <c r="H17" s="1"/>
-      <c r="I17">
-        <v>1.2096994127430401E-3</v>
-      </c>
+      <c r="I17" s="1"/>
       <c r="J17">
-        <v>5.9831239305520193E-4</v>
-      </c>
-      <c r="L17">
+        <v>4.9186014597573573</v>
+      </c>
+      <c r="K17">
+        <v>2.5495026984671894</v>
+      </c>
+      <c r="M17">
         <v>8.6852363282497586E-4</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>1.1323942888060183E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>3</v>
       </c>
-      <c r="C18">
-        <v>0.70489999999999997</v>
-      </c>
       <c r="D18">
-        <v>0.1449</v>
+        <v>0.49249999999999999</v>
       </c>
       <c r="E18">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="3"/>
-        <v>0.20556107249255215</v>
-      </c>
-      <c r="F18">
+        <v>9.8274111675126896E-2</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="4"/>
-        <v>4.8647342995169076</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>10.175619834710744</v>
+      </c>
       <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G16:G18"/>
     <mergeCell ref="H16:H18"/>
-    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="I16:I18"/>
     <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="I7:I9"/>
     <mergeCell ref="H10:H12"/>
-    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="I10:I12"/>
     <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4729,7 +4740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
poprawa współczynników - usunięcie błędów
</commit_message>
<xml_diff>
--- a/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
+++ b/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
@@ -172,11 +172,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80726656"/>
-        <c:axId val="81092992"/>
+        <c:axId val="69022464"/>
+        <c:axId val="69024000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80726656"/>
+        <c:axId val="69022464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -186,12 +186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81092992"/>
+        <c:crossAx val="69024000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81092992"/>
+        <c:axId val="69024000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -202,7 +202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80726656"/>
+        <c:crossAx val="69022464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -297,11 +297,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87152896"/>
-        <c:axId val="87158784"/>
+        <c:axId val="80706560"/>
+        <c:axId val="80724736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87152896"/>
+        <c:axId val="80706560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -311,12 +311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87158784"/>
+        <c:crossAx val="80724736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87158784"/>
+        <c:axId val="80724736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87152896"/>
+        <c:crossAx val="80706560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -422,11 +422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87203840"/>
-        <c:axId val="87205376"/>
+        <c:axId val="81089280"/>
+        <c:axId val="81090816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87203840"/>
+        <c:axId val="81089280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,12 +436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87205376"/>
+        <c:crossAx val="81090816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87205376"/>
+        <c:axId val="81090816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,14 +452,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87203840"/>
+        <c:crossAx val="81089280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -548,11 +547,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87225472"/>
-        <c:axId val="87227008"/>
+        <c:axId val="81127296"/>
+        <c:axId val="81128832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87225472"/>
+        <c:axId val="81127296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,12 +561,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87227008"/>
+        <c:crossAx val="81128832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87227008"/>
+        <c:axId val="81128832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -578,14 +577,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87225472"/>
+        <c:crossAx val="81127296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -674,11 +672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86792448"/>
-        <c:axId val="86806528"/>
+        <c:axId val="85138432"/>
+        <c:axId val="85152512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86792448"/>
+        <c:axId val="85138432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,12 +686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86806528"/>
+        <c:crossAx val="85152512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86806528"/>
+        <c:axId val="85152512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,14 +702,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86792448"/>
+        <c:crossAx val="85138432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -800,11 +797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85176704"/>
-        <c:axId val="85178240"/>
+        <c:axId val="86484480"/>
+        <c:axId val="86486400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85176704"/>
+        <c:axId val="86484480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,12 +811,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85178240"/>
+        <c:crossAx val="86486400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85178240"/>
+        <c:axId val="86486400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85176704"/>
+        <c:crossAx val="86484480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -925,11 +922,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85190144"/>
-        <c:axId val="85191680"/>
+        <c:axId val="93155328"/>
+        <c:axId val="93156864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85190144"/>
+        <c:axId val="93155328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,12 +936,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85191680"/>
+        <c:crossAx val="93156864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85191680"/>
+        <c:axId val="93156864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85190144"/>
+        <c:crossAx val="93155328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1050,11 +1047,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85232256"/>
-        <c:axId val="85234048"/>
+        <c:axId val="56872320"/>
+        <c:axId val="56878208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85232256"/>
+        <c:axId val="56872320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,12 +1061,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85234048"/>
+        <c:crossAx val="56878208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85234048"/>
+        <c:axId val="56878208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85232256"/>
+        <c:crossAx val="56872320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1175,11 +1172,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85275008"/>
-        <c:axId val="85276544"/>
+        <c:axId val="69063808"/>
+        <c:axId val="69065344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85275008"/>
+        <c:axId val="69063808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,12 +1186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85276544"/>
+        <c:crossAx val="69065344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85276544"/>
+        <c:axId val="69065344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85275008"/>
+        <c:crossAx val="69063808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1300,11 +1297,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85300736"/>
-        <c:axId val="85302272"/>
+        <c:axId val="69618304"/>
+        <c:axId val="69624192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85300736"/>
+        <c:axId val="69618304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1314,12 +1311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85302272"/>
+        <c:crossAx val="69624192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85302272"/>
+        <c:axId val="69624192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85300736"/>
+        <c:crossAx val="69618304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1425,11 +1422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87046400"/>
-        <c:axId val="87048192"/>
+        <c:axId val="69630976"/>
+        <c:axId val="69636864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87046400"/>
+        <c:axId val="69630976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,12 +1436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87048192"/>
+        <c:crossAx val="69636864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87048192"/>
+        <c:axId val="69636864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87046400"/>
+        <c:crossAx val="69630976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1550,11 +1547,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87105536"/>
-        <c:axId val="87107072"/>
+        <c:axId val="72016640"/>
+        <c:axId val="72018176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87105536"/>
+        <c:axId val="72016640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,12 +1561,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87107072"/>
+        <c:crossAx val="72018176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87107072"/>
+        <c:axId val="72018176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1577,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87105536"/>
+        <c:crossAx val="72016640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1675,11 +1672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87135360"/>
-        <c:axId val="87136896"/>
+        <c:axId val="80680832"/>
+        <c:axId val="80682368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87135360"/>
+        <c:axId val="80680832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,12 +1686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87136896"/>
+        <c:crossAx val="80682368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87136896"/>
+        <c:axId val="80682368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87135360"/>
+        <c:crossAx val="80680832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2431,7 +2428,7 @@
   <dimension ref="A5:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,18 +2660,18 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" ref="H13:I13" si="6">AVERAGE(E13:E15)</f>
-        <v>0.30336666666666662</v>
+        <v>0.22126666666666664</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="6"/>
-        <v>0.14142242882053521</v>
+        <v>9.8234632923638834E-2</v>
       </c>
       <c r="J13">
         <f t="array" ref="J13:K14">LINEST(D13:D15,E13:E15,TRUE,TRUE)</f>
-        <v>6.8309474156436458</v>
+        <v>10.203444546992337</v>
       </c>
       <c r="K13">
-        <v>0.18088491900757298</v>
+        <v>-4.5154967645042454E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2685,23 +2682,23 @@
         <v>1.901</v>
       </c>
       <c r="E14">
-        <v>0.43369999999999997</v>
+        <v>0.18740000000000001</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>0.2281430825881115</v>
+        <v>9.857969489742241E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>4.383214203366383</v>
+        <v>10.144076840981857</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14">
-        <v>5.6661812720707632</v>
+        <v>3.0144485209863715E-2</v>
       </c>
       <c r="K14">
-        <v>1.9998173602908687</v>
+        <v>8.1765355178919693E-3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2751,18 +2748,18 @@
       </c>
       <c r="H16" s="1">
         <f>AVERAGE(E16:E18)</f>
-        <v>0.42157</v>
+        <v>0.22146666666666667</v>
       </c>
       <c r="I16" s="1">
         <f>AVERAGE(F16:F18)</f>
-        <v>0.20354785230334607</v>
+        <v>9.827463400929444E-2</v>
       </c>
       <c r="J16">
         <f t="array" ref="J16:K17">LINEST(D16:D18,E16:E18,TRUE,TRUE)</f>
-        <v>1.9958488766515854</v>
+        <v>10.168456342562662</v>
       </c>
       <c r="K16">
-        <v>1.4117099890699909</v>
+        <v>1.1258686671222762E-3</v>
       </c>
       <c r="M16">
         <v>4.8571215441004565</v>
@@ -2779,23 +2776,23 @@
         <v>1.9008</v>
       </c>
       <c r="E17">
-        <v>0.78700999999999999</v>
+        <v>0.1867</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>0.41404145622895622</v>
+        <v>9.8221801346801349E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="4"/>
-        <v>2.4152170874575929</v>
+        <v>10.181039100160685</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17">
-        <v>4.9186014597573573</v>
+        <v>5.5628077818537036E-3</v>
       </c>
       <c r="K17">
-        <v>2.5495026984671894</v>
+        <v>1.5115352230104318E-3</v>
       </c>
       <c r="M17">
         <v>8.6852363282497586E-4</v>

</xml_diff>

<commit_message>
aktualizacja 2 kanałów dla drugiej płyty głównej
</commit_message>
<xml_diff>
--- a/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
+++ b/Dokumentacja/KALIBRACJA PLYTY GLOWNEJ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Glowna AC" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Karta 2 DC" sheetId="5" r:id="rId4"/>
     <sheet name="Karta 3 DC" sheetId="4" r:id="rId5"/>
     <sheet name="Karta 4 DC" sheetId="3" r:id="rId6"/>
+    <sheet name="Glowna AC - płyta 2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="8">
   <si>
     <t>in</t>
   </si>
@@ -172,11 +173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69022464"/>
-        <c:axId val="69024000"/>
+        <c:axId val="77777536"/>
+        <c:axId val="77816192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69022464"/>
+        <c:axId val="77777536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -186,12 +187,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69024000"/>
+        <c:crossAx val="77816192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69024000"/>
+        <c:axId val="77816192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -202,7 +203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69022464"/>
+        <c:crossAx val="77777536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -297,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80706560"/>
-        <c:axId val="80724736"/>
+        <c:axId val="81586432"/>
+        <c:axId val="81588224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80706560"/>
+        <c:axId val="81586432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -311,12 +312,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80724736"/>
+        <c:crossAx val="81588224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80724736"/>
+        <c:axId val="81588224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80706560"/>
+        <c:crossAx val="81586432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -422,11 +423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81089280"/>
-        <c:axId val="81090816"/>
+        <c:axId val="81633280"/>
+        <c:axId val="81634816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81089280"/>
+        <c:axId val="81633280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,12 +437,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81090816"/>
+        <c:crossAx val="81634816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81090816"/>
+        <c:axId val="81634816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +453,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81089280"/>
+        <c:crossAx val="81633280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -547,11 +548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81127296"/>
-        <c:axId val="81128832"/>
+        <c:axId val="81654912"/>
+        <c:axId val="81656448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81127296"/>
+        <c:axId val="81654912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,12 +562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81128832"/>
+        <c:crossAx val="81656448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81128832"/>
+        <c:axId val="81656448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81127296"/>
+        <c:crossAx val="81654912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -672,11 +673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85138432"/>
-        <c:axId val="85152512"/>
+        <c:axId val="86399232"/>
+        <c:axId val="86417408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85138432"/>
+        <c:axId val="86399232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,12 +687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85152512"/>
+        <c:crossAx val="86417408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85152512"/>
+        <c:axId val="86417408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85138432"/>
+        <c:crossAx val="86399232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -797,11 +798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86484480"/>
-        <c:axId val="86486400"/>
+        <c:axId val="79872384"/>
+        <c:axId val="79873920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86484480"/>
+        <c:axId val="79872384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,12 +812,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86486400"/>
+        <c:crossAx val="79873920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86486400"/>
+        <c:axId val="79873920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86484480"/>
+        <c:crossAx val="79872384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -922,11 +923,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93155328"/>
-        <c:axId val="93156864"/>
+        <c:axId val="79885824"/>
+        <c:axId val="79887360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93155328"/>
+        <c:axId val="79885824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +937,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93156864"/>
+        <c:crossAx val="79887360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93156864"/>
+        <c:axId val="79887360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93155328"/>
+        <c:crossAx val="79885824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1047,11 +1048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56872320"/>
-        <c:axId val="56878208"/>
+        <c:axId val="81758848"/>
+        <c:axId val="81760640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56872320"/>
+        <c:axId val="81758848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,12 +1062,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56878208"/>
+        <c:crossAx val="81760640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56878208"/>
+        <c:axId val="81760640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56872320"/>
+        <c:crossAx val="81758848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1172,11 +1173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69063808"/>
-        <c:axId val="69065344"/>
+        <c:axId val="86000384"/>
+        <c:axId val="86001920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69063808"/>
+        <c:axId val="86000384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,12 +1187,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69065344"/>
+        <c:crossAx val="86001920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69065344"/>
+        <c:axId val="86001920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,7 +1203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69063808"/>
+        <c:crossAx val="86000384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1297,11 +1298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69618304"/>
-        <c:axId val="69624192"/>
+        <c:axId val="86019456"/>
+        <c:axId val="86029440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69618304"/>
+        <c:axId val="86019456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,12 +1312,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69624192"/>
+        <c:crossAx val="86029440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69624192"/>
+        <c:axId val="86029440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,7 +1328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69618304"/>
+        <c:crossAx val="86019456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1422,11 +1423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69630976"/>
-        <c:axId val="69636864"/>
+        <c:axId val="81478016"/>
+        <c:axId val="81479552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69630976"/>
+        <c:axId val="81478016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,12 +1437,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69636864"/>
+        <c:crossAx val="81479552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69636864"/>
+        <c:axId val="81479552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +1453,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69630976"/>
+        <c:crossAx val="81478016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1547,11 +1548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72016640"/>
-        <c:axId val="72018176"/>
+        <c:axId val="86009728"/>
+        <c:axId val="81528320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72016640"/>
+        <c:axId val="86009728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,12 +1562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72018176"/>
+        <c:crossAx val="81528320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72018176"/>
+        <c:axId val="81528320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72016640"/>
+        <c:crossAx val="86009728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1672,11 +1673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80680832"/>
-        <c:axId val="80682368"/>
+        <c:axId val="81568896"/>
+        <c:axId val="81570432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80680832"/>
+        <c:axId val="81568896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,12 +1687,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80682368"/>
+        <c:crossAx val="81570432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80682368"/>
+        <c:axId val="81570432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80680832"/>
+        <c:crossAx val="81568896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2425,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:N18"/>
+  <dimension ref="A5:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2769,7 @@
         <v>-1.55928106662655E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>2</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>1.1323942888060183E-3</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>3</v>
       </c>
@@ -2822,8 +2823,296 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="e">
+        <f t="shared" ref="F19:F30" si="7">E19/D19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" t="e">
+        <f t="shared" ref="G19:G30" si="8">D19/E19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="1" t="e">
+        <f>AVERAGE(E19:E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="1" t="e">
+        <f>AVERAGE(F19:F21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" t="e">
+        <f t="array" ref="J19:K20">LINEST(D19:D21,E19:E21,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="1" t="e">
+        <f>AVERAGE(E22:E24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="1" t="e">
+        <f>AVERAGE(F22:F24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" t="e">
+        <f t="array" ref="J22:K23">LINEST(D22:D24,E22:E24,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="1" t="e">
+        <f>AVERAGE(E25:E27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="1" t="e">
+        <f>AVERAGE(F25:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f t="array" ref="J25:K26">LINEST(D25:D27,E25:E27,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="1" t="e">
+        <f>AVERAGE(E28:E30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="1" t="e">
+        <f>AVERAGE(F28:F30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="e">
+        <f t="array" ref="J28:K29">LINEST(D28:D30,E28:E30,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="I25:I27"/>
     <mergeCell ref="H16:H18"/>
     <mergeCell ref="I16:I18"/>
     <mergeCell ref="H7:H9"/>
@@ -5231,4 +5520,667 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:N30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>4.3650000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.42849999999999999</v>
+      </c>
+      <c r="F7">
+        <f>E7/D7</f>
+        <v>9.8167239404352805E-2</v>
+      </c>
+      <c r="G7">
+        <f>D7/E7</f>
+        <v>10.186697782963828</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:I7" si="0">AVERAGE(E7:E9)</f>
+        <v>0.21653</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>9.8134321767122237E-2</v>
+      </c>
+      <c r="J7">
+        <f t="array" ref="J7:K8">LINEST(D7:D9,E7:E9,TRUE,TRUE)</f>
+        <v>10.18588037308993</v>
+      </c>
+      <c r="K7">
+        <v>2.8465614817108076E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1.9008</v>
+      </c>
+      <c r="E8">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F30" si="1">E8/D8</f>
+        <v>9.8169191919191906E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G30" si="2">D8/E8</f>
+        <v>10.186495176848876</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8">
+        <v>7.470214409172715E-4</v>
+      </c>
+      <c r="K8">
+        <v>2.0212020868881717E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="E9">
+        <v>3.449E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>9.8066533977822001E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>10.197158596694695</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4.3650000000000002</v>
+      </c>
+      <c r="E10">
+        <v>0.43020000000000003</v>
+      </c>
+      <c r="F10">
+        <f>E12/D12</f>
+        <v>9.8321956769055724E-2</v>
+      </c>
+      <c r="G10">
+        <f>D12/E12</f>
+        <v>10.170668209430143</v>
+      </c>
+      <c r="H10" s="1">
+        <f>AVERAGE(E3:E11)</f>
+        <v>0.25759799999999999</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" ref="H10:I10" si="3">AVERAGE(F10:F12)</f>
+        <v>9.8487623689219081E-2</v>
+      </c>
+      <c r="J10" t="e">
+        <f t="array" ref="J10:K11">LINEST(D3:D11,E3:E11,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K10" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2.1118999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.2082</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>9.8584213267673665E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>10.143611911623438</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0.35160000000000002</v>
+      </c>
+      <c r="E12">
+        <v>3.4569999999999997E-2</v>
+      </c>
+      <c r="F12">
+        <f>E10/D10</f>
+        <v>9.855670103092784E-2</v>
+      </c>
+      <c r="G12">
+        <f>D10/E10</f>
+        <v>10.146443514644352</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="1" t="e">
+        <f t="shared" ref="H13:I13" si="4">AVERAGE(E13:E15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" t="e">
+        <f t="array" ref="J13:K14">LINEST(D13:D15,E13:E15,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="1" t="e">
+        <f>AVERAGE(E16:E18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="1" t="e">
+        <f>AVERAGE(F16:F18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" t="e">
+        <f t="array" ref="J16:K17">LINEST(D16:D18,E16:E18,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M16">
+        <v>4.8571215441004565</v>
+      </c>
+      <c r="N16">
+        <v>-1.55928106662655E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M17">
+        <v>8.6852363282497586E-4</v>
+      </c>
+      <c r="N17">
+        <v>1.1323942888060183E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="1" t="e">
+        <f>AVERAGE(E19:E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="1" t="e">
+        <f>AVERAGE(F19:F21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" t="e">
+        <f t="array" ref="J19:K20">LINEST(D19:D21,E19:E21,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="1" t="e">
+        <f>AVERAGE(E22:E24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="1" t="e">
+        <f>AVERAGE(F22:F24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" t="e">
+        <f t="array" ref="J22:K23">LINEST(D22:D24,E22:E24,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="1" t="e">
+        <f>AVERAGE(E25:E27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="1" t="e">
+        <f>AVERAGE(F25:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f t="array" ref="J25:K26">LINEST(D25:D27,E25:E27,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G28" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="1" t="e">
+        <f>AVERAGE(E28:E30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="1" t="e">
+        <f>AVERAGE(F28:F30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="e">
+        <f t="array" ref="J28:K29">LINEST(D28:D30,E28:E30,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" t="e">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>